<commit_message>
-A new column added for animal byproducts which because of regulations is sometimes required to know -A new option is the ability to download those chemicals marked as animal byproduct into a spreadsheet
</commit_message>
<xml_diff>
--- a/chemicalDB/data/chemicals-lab.xlsx
+++ b/chemicalDB/data/chemicals-lab.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Chemical.name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">exitDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnimalByproduct</t>
   </si>
   <si>
     <t xml:space="preserve">Potassium chloride</t>
@@ -200,9 +203,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P4" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:P4"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:Q4"/>
+  <tableColumns count="17">
     <tableColumn id="1" name="Chemical.name"/>
     <tableColumn id="2" name="SDS.sheet"/>
     <tableColumn id="3" name="CMR"/>
@@ -219,6 +222,7 @@
     <tableColumn id="14" name="Comments"/>
     <tableColumn id="15" name="entryDate"/>
     <tableColumn id="16" name="exitDate"/>
+    <tableColumn id="17" name="AnimalByproduct"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -507,7 +511,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -558,153 +562,165 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P3"/>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
+      <c r="Q4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>